<commit_message>
Modifying the cookbook parameters otherwise the compilation tests will fail.
</commit_message>
<xml_diff>
--- a/doc/user-guide/cookbook/rebalancing-requests/rebalancing-requests.xlsx
+++ b/doc/user-guide/cookbook/rebalancing-requests/rebalancing-requests.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\frepple-enterprise\doc\user-guide\cookbook\rebalancing-requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{38044A19-4964-4620-AB3B-348ECFCFD23A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5892" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5891" uniqueCount="1206">
   <si>
     <t>name</t>
   </si>
@@ -3056,12 +3057,6 @@
     <t>inventoryplanning.rebalancing_burnout_threshold</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>The minimum time to burn up excess inventory (compared to forecast) that can be rebalanced (in periods). If the burn out period (Excess Quantity/Forecast) is less than the threshold, the rebalancing will not occur. Default value: 0</t>
-  </si>
-  <si>
     <t>inventoryplanning.rebalancing_part_cost_threshold</t>
   </si>
   <si>
@@ -3654,12 +3649,15 @@
   </si>
   <si>
     <t>{'pegging': {'Umpire chair @ Tennis shop Paris - 2016-11-01': 0.151547, 'Umpire chair @ Tennis shop Paris - 2017-01-01': 0.315155, 'Umpire chair @ Tennis shop Paris - 2016-12-01': 0.315155}, 'location': 'Tennis shop Paris', 'item': 'Umpire chair'}</t>
+  </si>
+  <si>
+    <t>The minimum time to burn up excess inventory (compared to forecast) that can be rebalanced (in days If the burn out period (Excess Quantity/Forecast) is less than the threshold, the rebalancing will not occur. Default value: 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -3996,7 +3994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R763"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28449,7 +28447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28502,7 +28500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28560,7 +28558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28996,12 +28994,18 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="4" max="4" width="110.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -29682,11 +29686,11 @@
       <c r="A49" t="s">
         <v>1006</v>
       </c>
-      <c r="B49" t="s">
-        <v>1007</v>
+      <c r="B49">
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>1008</v>
+        <v>1205</v>
       </c>
       <c r="E49" s="1">
         <v>42835.589870630312</v>
@@ -29694,13 +29698,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B50" t="s">
         <v>995</v>
       </c>
       <c r="C50" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E50" s="1">
         <v>42835.589870700009</v>
@@ -29708,13 +29712,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C51" t="s">
         <v>1011</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1013</v>
       </c>
       <c r="E51" s="1">
         <v>42835.589870767733</v>
@@ -29722,13 +29726,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C52" t="s">
         <v>1014</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1016</v>
       </c>
       <c r="E52" s="1">
         <v>42835.589870834483</v>
@@ -29736,13 +29740,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C53" t="s">
         <v>1017</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1019</v>
       </c>
       <c r="E53" s="1">
         <v>42835.589870907177</v>
@@ -29750,13 +29754,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B54" t="s">
         <v>897</v>
       </c>
       <c r="C54" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E54" s="1">
         <v>42835.589870972937</v>
@@ -29764,13 +29768,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B55" t="s">
         <v>943</v>
       </c>
       <c r="C55" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E55" s="1">
         <v>42835.589871036689</v>
@@ -29778,13 +29782,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B56" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C56" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="E56" s="1">
         <v>42835.589871104152</v>
@@ -29792,13 +29796,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C57" t="s">
         <v>1026</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1028</v>
       </c>
       <c r="E57" s="1">
         <v>42835.589871166369</v>
@@ -29806,13 +29810,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B58" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="C58" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E58" s="1">
         <v>42835.589871230048</v>
@@ -29820,13 +29824,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C59" t="s">
         <v>1031</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1032</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1033</v>
       </c>
       <c r="E59" s="1">
         <v>42835.58987129767</v>
@@ -29834,10 +29838,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B60" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="E60" s="1">
         <v>42835.590324146542</v>
@@ -29849,7 +29853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29864,7 +29868,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -29878,7 +29882,7 @@
         <v>897</v>
       </c>
       <c r="B2" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -29893,7 +29897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29905,7 +29909,7 @@
         <v>848</v>
       </c>
       <c r="B1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -29931,7 +29935,7 @@
         <v>897</v>
       </c>
       <c r="C2" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D2" s="1">
         <v>40544</v>
@@ -29951,7 +29955,7 @@
         <v>897</v>
       </c>
       <c r="C3" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D3" s="1">
         <v>40575</v>
@@ -29971,7 +29975,7 @@
         <v>897</v>
       </c>
       <c r="C4" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D4" s="1">
         <v>40603</v>
@@ -29991,7 +29995,7 @@
         <v>897</v>
       </c>
       <c r="C5" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D5" s="1">
         <v>40634</v>
@@ -30011,7 +30015,7 @@
         <v>897</v>
       </c>
       <c r="C6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D6" s="1">
         <v>40664</v>
@@ -30031,7 +30035,7 @@
         <v>897</v>
       </c>
       <c r="C7" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D7" s="1">
         <v>40695</v>
@@ -30051,7 +30055,7 @@
         <v>897</v>
       </c>
       <c r="C8" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D8" s="1">
         <v>40725</v>
@@ -30071,7 +30075,7 @@
         <v>897</v>
       </c>
       <c r="C9" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D9" s="1">
         <v>40756</v>
@@ -30091,7 +30095,7 @@
         <v>897</v>
       </c>
       <c r="C10" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D10" s="1">
         <v>40787</v>
@@ -30111,7 +30115,7 @@
         <v>897</v>
       </c>
       <c r="C11" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D11" s="1">
         <v>40817</v>
@@ -30131,7 +30135,7 @@
         <v>897</v>
       </c>
       <c r="C12" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D12" s="1">
         <v>40848</v>
@@ -30151,7 +30155,7 @@
         <v>897</v>
       </c>
       <c r="C13" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D13" s="1">
         <v>40878</v>
@@ -30171,7 +30175,7 @@
         <v>897</v>
       </c>
       <c r="C14" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D14" s="1">
         <v>40909</v>
@@ -30191,7 +30195,7 @@
         <v>897</v>
       </c>
       <c r="C15" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="D15" s="1">
         <v>40940</v>
@@ -30211,7 +30215,7 @@
         <v>897</v>
       </c>
       <c r="C16" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D16" s="1">
         <v>40969</v>
@@ -30231,7 +30235,7 @@
         <v>897</v>
       </c>
       <c r="C17" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="D17" s="1">
         <v>41000</v>
@@ -30251,7 +30255,7 @@
         <v>897</v>
       </c>
       <c r="C18" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D18" s="1">
         <v>41030</v>
@@ -30271,7 +30275,7 @@
         <v>897</v>
       </c>
       <c r="C19" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="D19" s="1">
         <v>41061</v>
@@ -30291,7 +30295,7 @@
         <v>897</v>
       </c>
       <c r="C20" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D20" s="1">
         <v>41091</v>
@@ -30311,7 +30315,7 @@
         <v>897</v>
       </c>
       <c r="C21" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="D21" s="1">
         <v>41122</v>
@@ -30331,7 +30335,7 @@
         <v>897</v>
       </c>
       <c r="C22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D22" s="1">
         <v>41153</v>
@@ -30351,7 +30355,7 @@
         <v>897</v>
       </c>
       <c r="C23" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D23" s="1">
         <v>41183</v>
@@ -30371,7 +30375,7 @@
         <v>897</v>
       </c>
       <c r="C24" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D24" s="1">
         <v>41214</v>
@@ -30391,7 +30395,7 @@
         <v>897</v>
       </c>
       <c r="C25" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D25" s="1">
         <v>41244</v>
@@ -30411,7 +30415,7 @@
         <v>897</v>
       </c>
       <c r="C26" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D26" s="1">
         <v>41275</v>
@@ -30431,7 +30435,7 @@
         <v>897</v>
       </c>
       <c r="C27" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="D27" s="1">
         <v>41306</v>
@@ -30451,7 +30455,7 @@
         <v>897</v>
       </c>
       <c r="C28" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D28" s="1">
         <v>41334</v>
@@ -30471,7 +30475,7 @@
         <v>897</v>
       </c>
       <c r="C29" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="D29" s="1">
         <v>41365</v>
@@ -30491,7 +30495,7 @@
         <v>897</v>
       </c>
       <c r="C30" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D30" s="1">
         <v>41395</v>
@@ -30511,7 +30515,7 @@
         <v>897</v>
       </c>
       <c r="C31" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D31" s="1">
         <v>41426</v>
@@ -30531,7 +30535,7 @@
         <v>897</v>
       </c>
       <c r="C32" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D32" s="1">
         <v>41456</v>
@@ -30551,7 +30555,7 @@
         <v>897</v>
       </c>
       <c r="C33" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="D33" s="1">
         <v>41487</v>
@@ -30571,7 +30575,7 @@
         <v>897</v>
       </c>
       <c r="C34" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D34" s="1">
         <v>41518</v>
@@ -30591,7 +30595,7 @@
         <v>897</v>
       </c>
       <c r="C35" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="D35" s="1">
         <v>41548</v>
@@ -30611,7 +30615,7 @@
         <v>897</v>
       </c>
       <c r="C36" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D36" s="1">
         <v>41579</v>
@@ -30631,7 +30635,7 @@
         <v>897</v>
       </c>
       <c r="C37" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="D37" s="1">
         <v>41609</v>
@@ -30651,7 +30655,7 @@
         <v>897</v>
       </c>
       <c r="C38" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D38" s="1">
         <v>41640</v>
@@ -30671,7 +30675,7 @@
         <v>897</v>
       </c>
       <c r="C39" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="D39" s="1">
         <v>41671</v>
@@ -30691,7 +30695,7 @@
         <v>897</v>
       </c>
       <c r="C40" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D40" s="1">
         <v>41699</v>
@@ -30711,7 +30715,7 @@
         <v>897</v>
       </c>
       <c r="C41" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="D41" s="1">
         <v>41730</v>
@@ -30731,7 +30735,7 @@
         <v>897</v>
       </c>
       <c r="C42" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D42" s="1">
         <v>41760</v>
@@ -30751,7 +30755,7 @@
         <v>897</v>
       </c>
       <c r="C43" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D43" s="1">
         <v>41791</v>
@@ -30771,7 +30775,7 @@
         <v>897</v>
       </c>
       <c r="C44" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="D44" s="1">
         <v>41821</v>
@@ -30791,7 +30795,7 @@
         <v>897</v>
       </c>
       <c r="C45" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D45" s="1">
         <v>41852</v>
@@ -30811,7 +30815,7 @@
         <v>897</v>
       </c>
       <c r="C46" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D46" s="1">
         <v>41883</v>
@@ -30831,7 +30835,7 @@
         <v>897</v>
       </c>
       <c r="C47" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D47" s="1">
         <v>41913</v>
@@ -30851,7 +30855,7 @@
         <v>897</v>
       </c>
       <c r="C48" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="D48" s="1">
         <v>41944</v>
@@ -30871,7 +30875,7 @@
         <v>897</v>
       </c>
       <c r="C49" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D49" s="1">
         <v>41974</v>
@@ -30891,7 +30895,7 @@
         <v>897</v>
       </c>
       <c r="C50" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="D50" s="1">
         <v>42005</v>
@@ -30911,7 +30915,7 @@
         <v>897</v>
       </c>
       <c r="C51" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D51" s="1">
         <v>42036</v>
@@ -30931,7 +30935,7 @@
         <v>897</v>
       </c>
       <c r="C52" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="D52" s="1">
         <v>42064</v>
@@ -30951,7 +30955,7 @@
         <v>897</v>
       </c>
       <c r="C53" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D53" s="1">
         <v>42095</v>
@@ -30971,7 +30975,7 @@
         <v>897</v>
       </c>
       <c r="C54" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D54" s="1">
         <v>42125</v>
@@ -30991,7 +30995,7 @@
         <v>897</v>
       </c>
       <c r="C55" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D55" s="1">
         <v>42156</v>
@@ -31011,7 +31015,7 @@
         <v>897</v>
       </c>
       <c r="C56" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D56" s="1">
         <v>42186</v>
@@ -31031,7 +31035,7 @@
         <v>897</v>
       </c>
       <c r="C57" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D57" s="1">
         <v>42217</v>
@@ -31051,7 +31055,7 @@
         <v>897</v>
       </c>
       <c r="C58" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="D58" s="1">
         <v>42248</v>
@@ -31071,7 +31075,7 @@
         <v>897</v>
       </c>
       <c r="C59" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D59" s="1">
         <v>42278</v>
@@ -31091,7 +31095,7 @@
         <v>897</v>
       </c>
       <c r="C60" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="D60" s="1">
         <v>42309</v>
@@ -31111,7 +31115,7 @@
         <v>897</v>
       </c>
       <c r="C61" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D61" s="1">
         <v>42339</v>
@@ -31131,7 +31135,7 @@
         <v>897</v>
       </c>
       <c r="C62" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="D62" s="1">
         <v>42370</v>
@@ -31151,7 +31155,7 @@
         <v>897</v>
       </c>
       <c r="C63" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D63" s="1">
         <v>42401</v>
@@ -31171,7 +31175,7 @@
         <v>897</v>
       </c>
       <c r="C64" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="D64" s="1">
         <v>42430</v>
@@ -31191,7 +31195,7 @@
         <v>897</v>
       </c>
       <c r="C65" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D65" s="1">
         <v>42461</v>
@@ -31211,7 +31215,7 @@
         <v>897</v>
       </c>
       <c r="C66" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D66" s="1">
         <v>42491</v>
@@ -31231,7 +31235,7 @@
         <v>897</v>
       </c>
       <c r="C67" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="D67" s="1">
         <v>42522</v>
@@ -31251,7 +31255,7 @@
         <v>897</v>
       </c>
       <c r="C68" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D68" s="1">
         <v>42552</v>
@@ -31271,7 +31275,7 @@
         <v>897</v>
       </c>
       <c r="C69" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D69" s="1">
         <v>42583</v>
@@ -31291,7 +31295,7 @@
         <v>897</v>
       </c>
       <c r="C70" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D70" s="1">
         <v>42614</v>
@@ -31311,7 +31315,7 @@
         <v>897</v>
       </c>
       <c r="C71" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="D71" s="1">
         <v>42644</v>
@@ -31331,7 +31335,7 @@
         <v>897</v>
       </c>
       <c r="C72" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D72" s="1">
         <v>42675</v>
@@ -31351,7 +31355,7 @@
         <v>897</v>
       </c>
       <c r="C73" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D73" s="1">
         <v>42705</v>
@@ -31371,7 +31375,7 @@
         <v>897</v>
       </c>
       <c r="C74" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D74" s="1">
         <v>42736</v>
@@ -31391,7 +31395,7 @@
         <v>897</v>
       </c>
       <c r="C75" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D75" s="1">
         <v>42767</v>
@@ -31411,7 +31415,7 @@
         <v>897</v>
       </c>
       <c r="C76" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D76" s="1">
         <v>42795</v>
@@ -31431,7 +31435,7 @@
         <v>897</v>
       </c>
       <c r="C77" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D77" s="1">
         <v>42826</v>
@@ -31451,7 +31455,7 @@
         <v>897</v>
       </c>
       <c r="C78" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D78" s="1">
         <v>42856</v>
@@ -31471,7 +31475,7 @@
         <v>897</v>
       </c>
       <c r="C79" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D79" s="1">
         <v>42887</v>
@@ -31491,7 +31495,7 @@
         <v>897</v>
       </c>
       <c r="C80" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="D80" s="1">
         <v>42917</v>
@@ -31511,7 +31515,7 @@
         <v>897</v>
       </c>
       <c r="C81" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D81" s="1">
         <v>42948</v>
@@ -31531,7 +31535,7 @@
         <v>897</v>
       </c>
       <c r="C82" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D82" s="1">
         <v>42979</v>
@@ -31551,7 +31555,7 @@
         <v>897</v>
       </c>
       <c r="C83" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D83" s="1">
         <v>43009</v>
@@ -31571,7 +31575,7 @@
         <v>897</v>
       </c>
       <c r="C84" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D84" s="1">
         <v>43040</v>
@@ -31591,7 +31595,7 @@
         <v>897</v>
       </c>
       <c r="C85" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="D85" s="1">
         <v>43070</v>
@@ -31611,7 +31615,7 @@
         <v>897</v>
       </c>
       <c r="C86" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D86" s="1">
         <v>43101</v>
@@ -31631,7 +31635,7 @@
         <v>897</v>
       </c>
       <c r="C87" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D87" s="1">
         <v>43132</v>
@@ -31651,7 +31655,7 @@
         <v>897</v>
       </c>
       <c r="C88" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D88" s="1">
         <v>43160</v>
@@ -31671,7 +31675,7 @@
         <v>897</v>
       </c>
       <c r="C89" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="D89" s="1">
         <v>43191</v>
@@ -31691,7 +31695,7 @@
         <v>897</v>
       </c>
       <c r="C90" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D90" s="1">
         <v>43221</v>
@@ -31711,7 +31715,7 @@
         <v>897</v>
       </c>
       <c r="C91" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="D91" s="1">
         <v>43252</v>
@@ -31731,7 +31735,7 @@
         <v>897</v>
       </c>
       <c r="C92" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D92" s="1">
         <v>43282</v>
@@ -31751,7 +31755,7 @@
         <v>897</v>
       </c>
       <c r="C93" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="D93" s="1">
         <v>43313</v>
@@ -31771,7 +31775,7 @@
         <v>897</v>
       </c>
       <c r="C94" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D94" s="1">
         <v>43344</v>
@@ -31791,7 +31795,7 @@
         <v>897</v>
       </c>
       <c r="C95" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="D95" s="1">
         <v>43374</v>
@@ -31811,7 +31815,7 @@
         <v>897</v>
       </c>
       <c r="C96" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D96" s="1">
         <v>43405</v>
@@ -31831,7 +31835,7 @@
         <v>897</v>
       </c>
       <c r="C97" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="D97" s="1">
         <v>43435</v>
@@ -31849,7 +31853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32147,7 +32151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32239,7 +32243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32283,7 +32287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33119,10 +33123,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -33189,7 +33193,7 @@
         <v>42404</v>
       </c>
       <c r="H2" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="I2" t="s">
         <v>372</v>
@@ -33224,7 +33228,7 @@
         <v>42404</v>
       </c>
       <c r="H3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="I3" t="s">
         <v>61</v>
@@ -33259,7 +33263,7 @@
         <v>42404</v>
       </c>
       <c r="H4" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="I4" t="s">
         <v>289</v>
@@ -33294,7 +33298,7 @@
         <v>42411</v>
       </c>
       <c r="H5" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
@@ -33329,7 +33333,7 @@
         <v>42522</v>
       </c>
       <c r="H6" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I6" t="s">
         <v>20</v>
@@ -33364,7 +33368,7 @@
         <v>42736</v>
       </c>
       <c r="H7" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="I7" t="s">
         <v>20</v>
@@ -33399,7 +33403,7 @@
         <v>42411</v>
       </c>
       <c r="H8" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="I8" t="s">
         <v>20</v>
@@ -33434,7 +33438,7 @@
         <v>42522</v>
       </c>
       <c r="H9" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="I9" t="s">
         <v>20</v>
@@ -33469,7 +33473,7 @@
         <v>42522</v>
       </c>
       <c r="H10" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="I10" t="s">
         <v>61</v>
@@ -33504,7 +33508,7 @@
         <v>42407</v>
       </c>
       <c r="H11" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="I11" t="s">
         <v>61</v>
@@ -33539,7 +33543,7 @@
         <v>42522</v>
       </c>
       <c r="H12" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="I12" t="s">
         <v>61</v>
@@ -33574,7 +33578,7 @@
         <v>42705</v>
       </c>
       <c r="H13" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="I13" t="s">
         <v>61</v>
@@ -33609,7 +33613,7 @@
         <v>42522</v>
       </c>
       <c r="H14" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="I14" t="s">
         <v>99</v>
@@ -33644,7 +33648,7 @@
         <v>42430</v>
       </c>
       <c r="H15" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="I15" t="s">
         <v>99</v>
@@ -33679,7 +33683,7 @@
         <v>42491</v>
       </c>
       <c r="H16" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="I16" t="s">
         <v>99</v>
@@ -33714,7 +33718,7 @@
         <v>42414</v>
       </c>
       <c r="H17" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="I17" t="s">
         <v>137</v>
@@ -33749,7 +33753,7 @@
         <v>42644</v>
       </c>
       <c r="H18" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="I18" t="s">
         <v>137</v>
@@ -33784,7 +33788,7 @@
         <v>42414</v>
       </c>
       <c r="H19" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="I19" t="s">
         <v>137</v>
@@ -33819,7 +33823,7 @@
         <v>42552</v>
       </c>
       <c r="H20" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="I20" t="s">
         <v>137</v>
@@ -33854,7 +33858,7 @@
         <v>42411</v>
       </c>
       <c r="H21" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="I21" t="s">
         <v>175</v>
@@ -33889,7 +33893,7 @@
         <v>42583</v>
       </c>
       <c r="H22" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="I22" t="s">
         <v>175</v>
@@ -33924,7 +33928,7 @@
         <v>42411</v>
       </c>
       <c r="H23" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="I23" t="s">
         <v>175</v>
@@ -33959,7 +33963,7 @@
         <v>42407</v>
       </c>
       <c r="H24" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="I24" t="s">
         <v>372</v>
@@ -33994,7 +33998,7 @@
         <v>42430</v>
       </c>
       <c r="H25" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="I25" t="s">
         <v>372</v>
@@ -34029,7 +34033,7 @@
         <v>42461</v>
       </c>
       <c r="H26" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="I26" t="s">
         <v>372</v>
@@ -34064,7 +34068,7 @@
         <v>42491</v>
       </c>
       <c r="H27" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="I27" t="s">
         <v>372</v>
@@ -34099,7 +34103,7 @@
         <v>42522</v>
       </c>
       <c r="H28" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="I28" t="s">
         <v>372</v>
@@ -34134,7 +34138,7 @@
         <v>42552</v>
       </c>
       <c r="H29" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="I29" t="s">
         <v>372</v>
@@ -34169,7 +34173,7 @@
         <v>42583</v>
       </c>
       <c r="H30" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="I30" t="s">
         <v>372</v>
@@ -34204,7 +34208,7 @@
         <v>42614</v>
       </c>
       <c r="H31" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="I31" t="s">
         <v>372</v>
@@ -34239,7 +34243,7 @@
         <v>42644</v>
       </c>
       <c r="H32" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="I32" t="s">
         <v>372</v>
@@ -34274,7 +34278,7 @@
         <v>42675</v>
       </c>
       <c r="H33" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="I33" t="s">
         <v>372</v>
@@ -34309,7 +34313,7 @@
         <v>42705</v>
       </c>
       <c r="H34" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="I34" t="s">
         <v>372</v>
@@ -34344,7 +34348,7 @@
         <v>42736</v>
       </c>
       <c r="H35" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="I35" t="s">
         <v>372</v>
@@ -34379,7 +34383,7 @@
         <v>42430</v>
       </c>
       <c r="H36" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="I36" t="s">
         <v>372</v>
@@ -34414,7 +34418,7 @@
         <v>42461</v>
       </c>
       <c r="H37" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="I37" t="s">
         <v>372</v>
@@ -34449,7 +34453,7 @@
         <v>42491</v>
       </c>
       <c r="H38" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="I38" t="s">
         <v>372</v>
@@ -34484,7 +34488,7 @@
         <v>42522</v>
       </c>
       <c r="H39" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="I39" t="s">
         <v>372</v>
@@ -34519,7 +34523,7 @@
         <v>42552</v>
       </c>
       <c r="H40" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="I40" t="s">
         <v>372</v>
@@ -34554,7 +34558,7 @@
         <v>42583</v>
       </c>
       <c r="H41" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="I41" t="s">
         <v>372</v>
@@ -34589,7 +34593,7 @@
         <v>42614</v>
       </c>
       <c r="H42" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="I42" t="s">
         <v>372</v>
@@ -34624,7 +34628,7 @@
         <v>42644</v>
       </c>
       <c r="H43" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="I43" t="s">
         <v>372</v>
@@ -34659,7 +34663,7 @@
         <v>42675</v>
       </c>
       <c r="H44" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="I44" t="s">
         <v>372</v>
@@ -34694,7 +34698,7 @@
         <v>42705</v>
       </c>
       <c r="H45" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="I45" t="s">
         <v>372</v>
@@ -34729,7 +34733,7 @@
         <v>42736</v>
       </c>
       <c r="H46" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="I46" t="s">
         <v>372</v>
@@ -34764,7 +34768,7 @@
         <v>42419</v>
       </c>
       <c r="H47" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="I47" t="s">
         <v>327</v>
@@ -34799,7 +34803,7 @@
         <v>42419</v>
       </c>
       <c r="H48" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="I48" t="s">
         <v>327</v>
@@ -34834,7 +34838,7 @@
         <v>42736</v>
       </c>
       <c r="H49" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="I49" t="s">
         <v>327</v>
@@ -34869,7 +34873,7 @@
         <v>42425</v>
       </c>
       <c r="H50" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="I50" t="s">
         <v>213</v>
@@ -34904,7 +34908,7 @@
         <v>42491</v>
       </c>
       <c r="H51" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="I51" t="s">
         <v>213</v>
@@ -34939,7 +34943,7 @@
         <v>42522</v>
       </c>
       <c r="H52" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="I52" t="s">
         <v>213</v>
@@ -34974,7 +34978,7 @@
         <v>42552</v>
       </c>
       <c r="H53" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="I53" t="s">
         <v>213</v>
@@ -35009,7 +35013,7 @@
         <v>42675</v>
       </c>
       <c r="H54" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="I54" t="s">
         <v>213</v>
@@ -35044,7 +35048,7 @@
         <v>42425</v>
       </c>
       <c r="H55" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="I55" t="s">
         <v>213</v>
@@ -35079,7 +35083,7 @@
         <v>42491</v>
       </c>
       <c r="H56" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="I56" t="s">
         <v>213</v>
@@ -35114,7 +35118,7 @@
         <v>42522</v>
       </c>
       <c r="H57" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="I57" t="s">
         <v>213</v>
@@ -35149,7 +35153,7 @@
         <v>42552</v>
       </c>
       <c r="H58" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="I58" t="s">
         <v>213</v>
@@ -35184,7 +35188,7 @@
         <v>42644</v>
       </c>
       <c r="H59" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="I59" t="s">
         <v>213</v>
@@ -35219,7 +35223,7 @@
         <v>42419</v>
       </c>
       <c r="H60" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="I60" t="s">
         <v>251</v>
@@ -35254,7 +35258,7 @@
         <v>42522</v>
       </c>
       <c r="H61" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="I61" t="s">
         <v>251</v>
@@ -35289,7 +35293,7 @@
         <v>42705</v>
       </c>
       <c r="H62" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="I62" t="s">
         <v>251</v>
@@ -35324,7 +35328,7 @@
         <v>42419</v>
       </c>
       <c r="H63" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="I63" t="s">
         <v>251</v>
@@ -35359,7 +35363,7 @@
         <v>42522</v>
       </c>
       <c r="H64" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="I64" t="s">
         <v>251</v>
@@ -35394,7 +35398,7 @@
         <v>42583</v>
       </c>
       <c r="H65" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="I65" t="s">
         <v>251</v>
@@ -35429,7 +35433,7 @@
         <v>42522</v>
       </c>
       <c r="H66" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I66" t="s">
         <v>289</v>
@@ -35464,7 +35468,7 @@
         <v>42583</v>
       </c>
       <c r="H67" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I67" t="s">
         <v>289</v>
@@ -35499,7 +35503,7 @@
         <v>42419</v>
       </c>
       <c r="H68" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="I68" t="s">
         <v>289</v>
@@ -35534,7 +35538,7 @@
         <v>42522</v>
       </c>
       <c r="H69" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="I69" t="s">
         <v>289</v>
@@ -35569,7 +35573,7 @@
         <v>42425</v>
       </c>
       <c r="H70" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="I70" t="s">
         <v>365</v>
@@ -35604,7 +35608,7 @@
         <v>42583</v>
       </c>
       <c r="H71" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="I71" t="s">
         <v>365</v>
@@ -35639,7 +35643,7 @@
         <v>42404</v>
       </c>
       <c r="H72" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="I72" t="s">
         <v>365</v>
@@ -35674,7 +35678,7 @@
         <v>42583</v>
       </c>
       <c r="H73" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="I73" t="s">
         <v>365</v>
@@ -35695,7 +35699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36511,7 +36515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37212,7 +37216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>